<commit_message>
Adds shp file and logic for that in document
</commit_message>
<xml_diff>
--- a/data-raw/mandy-salmanid-habitat-monitoring/Enclosure Study - Growth Rates/enclosure-study-growth-rates-metadata.xlsx
+++ b/data-raw/mandy-salmanid-habitat-monitoring/Enclosure Study - Growth Rates/enclosure-study-growth-rates-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA_Salmonid_Habitat_Monitoring\data-raw\mandy-salmanid-habitat-monitoring\Enclosure Study - Growth Rates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6522931-1533-4A55-B159-6010C2234DB8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C5FA35-7059-4D0E-8BAC-7E1ACFB7FDC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10080" yWindow="-16560" windowWidth="29040" windowHeight="15840" tabRatio="834" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="834" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="143">
   <si>
     <t>first_name</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>day</t>
+  </si>
+  <si>
+    <t>CVPIA</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMH16384"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -53172,10 +53175,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -53210,6 +53213,11 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds required metadata info to metadata
</commit_message>
<xml_diff>
--- a/data-raw/mandy-salmanid-habitat-monitoring/Enclosure Study - Growth Rates/enclosure-study-growth-rates-metadata.xlsx
+++ b/data-raw/mandy-salmanid-habitat-monitoring/Enclosure Study - Growth Rates/enclosure-study-growth-rates-metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA_Salmonid_Habitat_Monitoring\data-raw\mandy-salmanid-habitat-monitoring\Enclosure Study - Growth Rates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C5FA35-7059-4D0E-8BAC-7E1ACFB7FDC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C599064-0CED-427F-A36B-D6C9F1E8F880}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="834" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26220" yWindow="-14385" windowWidth="15375" windowHeight="7875" tabRatio="834" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="13" r:id="rId1"/>
@@ -314,16 +314,10 @@
     <t>CVPIA Salmonid Monitoring Habitat Project</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Salmonid Spawning and Rearing Habitat Restoration in the Sacramento River</t>
   </si>
   <si>
     <t>ongoing</t>
-  </si>
-  <si>
-    <t>Bureau of Reclamation</t>
   </si>
   <si>
     <t>Sacramento Riverin northern California in the reach of the river between Keswick Dam and Sacramento</t>
@@ -466,6 +460,12 @@
   <si>
     <t>CVPIA</t>
   </si>
+  <si>
+    <t>USBR</t>
+  </si>
+  <si>
+    <t>R14AC00096</t>
+  </si>
 </sst>
 </file>
 
@@ -474,7 +474,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -497,6 +497,12 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -512,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -520,12 +526,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF8EA9DB"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -557,6 +572,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1035,12 +1053,12 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1127,20 +1145,20 @@
     </row>
     <row r="2" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1153,20 +1171,20 @@
     </row>
     <row r="3" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1179,29 +1197,29 @@
     </row>
     <row r="4" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="12"/>
@@ -1215,29 +1233,29 @@
     </row>
     <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="12"/>
@@ -1251,29 +1269,29 @@
     </row>
     <row r="6" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J6" s="13"/>
       <c r="K6" s="12"/>
@@ -1287,29 +1305,29 @@
     </row>
     <row r="7" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J7" s="13"/>
       <c r="K7" s="12"/>
@@ -1323,29 +1341,29 @@
     </row>
     <row r="8" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="12"/>
@@ -1359,29 +1377,29 @@
     </row>
     <row r="9" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="12"/>
@@ -1395,29 +1413,29 @@
     </row>
     <row r="10" spans="1:14" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="12"/>
@@ -1431,29 +1449,29 @@
     </row>
     <row r="11" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="12"/>
@@ -1467,29 +1485,29 @@
     </row>
     <row r="12" spans="1:14" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J12" s="13"/>
       <c r="K12" s="12"/>
@@ -1503,20 +1521,20 @@
     </row>
     <row r="13" spans="1:14" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
@@ -1529,20 +1547,20 @@
     </row>
     <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
@@ -1555,29 +1573,29 @@
     </row>
     <row r="15" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J15" s="13"/>
       <c r="K15" s="12"/>
@@ -53161,7 +53179,7 @@
     </row>
     <row r="2" spans="1:2" ht="114.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
         <v>84</v>
@@ -53177,7 +53195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -53217,7 +53235,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -53358,8 +53376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -53392,16 +53410,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
@@ -53414,7 +53432,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -53441,10 +53459,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -53508,7 +53526,7 @@
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B2" s="1">
         <v>-122.448217</v>

</xml_diff>